<commit_message>
Server to client broadcasts for day
</commit_message>
<xml_diff>
--- a/Api.xlsx
+++ b/Api.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="110">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -289,6 +289,12 @@
     <t xml:space="preserve">voteReady</t>
   </si>
   <si>
+    <t xml:space="preserve">Vote Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voteStart</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vote</t>
   </si>
   <si>
@@ -298,6 +304,18 @@
     <t xml:space="preserve">Player ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Vote Received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voteReceived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">playerID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player ID that sent the vote; broadcast to all</t>
+  </si>
+  <si>
     <t xml:space="preserve">Result</t>
   </si>
   <si>
@@ -307,7 +325,7 @@
     <t xml:space="preserve">votes, playerRoles, winTeam</t>
   </si>
   <si>
-    <t xml:space="preserve">Votes = map from id to votes, playerRoles = map from id to roles, winTeam = id</t>
+    <t xml:space="preserve">Votes = array from id to votes, playerRoles = array from id to roles, winTeam = id</t>
   </si>
   <si>
     <t xml:space="preserve">New Game</t>
@@ -455,10 +473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -851,74 +869,96 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="C35" s="0" t="s">
         <v>89</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E35" s="0" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="0" t="s">
+      <c r="F36" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="0" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="D37" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="E37" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="0" t="s">
+      <c r="C38" s="0" t="s">
         <v>98</v>
       </c>
+      <c r="D38" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="A40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>103</v>
+      <c r="F42" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +967,7 @@
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Day phase no ready-up
</commit_message>
<xml_diff>
--- a/Api.xlsx
+++ b/Api.xlsx
@@ -325,7 +325,7 @@
     <t xml:space="preserve">votes, playerRoles, winTeam</t>
   </si>
   <si>
-    <t xml:space="preserve">Votes = array from id to votes, playerRoles = array from id to roles, winTeam = id</t>
+    <t xml:space="preserve">Votes = array from id to votes, playerRoles = array from id to roles, winTeam = id[]</t>
   </si>
   <si>
     <t xml:space="preserve">New Game</t>
@@ -479,7 +479,7 @@
       <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>

</xml_diff>

<commit_message>
Handle Disconnects; Server Complete?
</commit_message>
<xml_diff>
--- a/Api.xlsx
+++ b/Api.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="110">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t xml:space="preserve">Restarting game; expect to follow with setupStart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disconnect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disconn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End game</t>
   </si>
 </sst>
 </file>
@@ -464,10 +473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -953,6 +962,17 @@
       </c>
       <c r="F43" s="0" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>